<commit_message>
Movement wurde inklusive Kommentar zum Code wurde hinzugefügt
</commit_message>
<xml_diff>
--- a/doc/Zeitplanung.xlsx
+++ b/doc/Zeitplanung.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="DieseArbeitsmappe" showPivotChartFilter="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\royal\Documents\_Basislehrjahr\__ProjektArbeit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Jump-And-Run\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFECC944-6F1A-4DFF-980C-292AA9E8230A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD199AF-ACA4-43EA-B9DD-A180336973AF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1640,7 +1640,7 @@
                   <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2147,8 +2147,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AN21" sqref="AN21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3422,7 +3422,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3495,7 +3495,7 @@
       </c>
       <c r="D19" s="83">
         <f>SUM(G19:BJ19)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19" s="50"/>
       <c r="F19" s="51"/>
@@ -3508,9 +3508,7 @@
       <c r="M19" s="58"/>
       <c r="N19" s="53"/>
       <c r="O19" s="54"/>
-      <c r="P19" s="89">
-        <v>1</v>
-      </c>
+      <c r="P19" s="89"/>
       <c r="Q19" s="55"/>
       <c r="R19" s="56"/>
       <c r="S19" s="57"/>
@@ -3570,7 +3568,7 @@
       </c>
       <c r="D20" s="83">
         <f t="shared" ref="D20:D30" si="0">SUM(G20:BJ20)</f>
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="E20" s="50"/>
       <c r="F20" s="51"/>
@@ -3584,7 +3582,7 @@
       <c r="N20" s="59"/>
       <c r="O20" s="60"/>
       <c r="P20" s="89">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="Q20" s="89"/>
       <c r="R20" s="91"/>
@@ -3645,7 +3643,7 @@
       </c>
       <c r="D21" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E21" s="50"/>
       <c r="F21" s="52" t="s">
@@ -3660,7 +3658,9 @@
       <c r="M21" s="58"/>
       <c r="N21" s="59"/>
       <c r="O21" s="60"/>
-      <c r="P21" s="93"/>
+      <c r="P21" s="93">
+        <v>4</v>
+      </c>
       <c r="Q21" s="89"/>
       <c r="R21" s="52"/>
       <c r="S21" s="57"/>
@@ -5243,7 +5243,7 @@
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>16.5</v>
+        <v>18</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5285,7 +5285,7 @@
       </c>
       <c r="P43" s="39">
         <f t="shared" si="3"/>
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="Q43" s="39">
         <f t="shared" si="3"/>
@@ -5575,7 +5575,7 @@
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>4.5</v>
+        <v>6</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>

</xml_diff>

<commit_message>
erstes "Hindernis" wurde hinzugefügt.
</commit_message>
<xml_diff>
--- a/doc/Zeitplanung.xlsx
+++ b/doc/Zeitplanung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Jump-And-Run\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD199AF-ACA4-43EA-B9DD-A180336973AF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8EDAA55-C929-4B39-9F95-110008F9AF1A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1640,7 +1640,7 @@
                   <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>6.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2148,7 +2148,7 @@
   <dimension ref="A1:BJ43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3422,7 +3422,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>6</v>
+        <v>6.25</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3643,7 +3643,7 @@
       </c>
       <c r="D21" s="83">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>4.25</v>
       </c>
       <c r="E21" s="50"/>
       <c r="F21" s="52" t="s">
@@ -3659,7 +3659,7 @@
       <c r="N21" s="59"/>
       <c r="O21" s="60"/>
       <c r="P21" s="93">
-        <v>4</v>
+        <v>4.25</v>
       </c>
       <c r="Q21" s="89"/>
       <c r="R21" s="52"/>
@@ -5243,7 +5243,7 @@
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>18</v>
+        <v>18.25</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5285,7 +5285,7 @@
       </c>
       <c r="P43" s="39">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>6.25</v>
       </c>
       <c r="Q43" s="39">
         <f t="shared" si="3"/>
@@ -5575,7 +5575,7 @@
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>6</v>
+        <v>6.25</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>

</xml_diff>

<commit_message>
Drei temporäre Hindernisse wurden in das Spiel integriert. Ebenfalls wurde die Anforderung der Musik noch realisiert.
</commit_message>
<xml_diff>
--- a/doc/Zeitplanung.xlsx
+++ b/doc/Zeitplanung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Jump-And-Run\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8EDAA55-C929-4B39-9F95-110008F9AF1A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8EC601A-95DD-4B9E-ADB3-126762A3ED0F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1640,7 +1640,7 @@
                   <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.25</c:v>
+                  <c:v>10.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2148,7 +2148,7 @@
   <dimension ref="A1:BJ43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3422,7 +3422,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>6.25</v>
+        <v>10.25</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3568,7 +3568,7 @@
       </c>
       <c r="D20" s="83">
         <f t="shared" ref="D20:D30" si="0">SUM(G20:BJ20)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E20" s="50"/>
       <c r="F20" s="51"/>
@@ -3584,7 +3584,9 @@
       <c r="P20" s="89">
         <v>2</v>
       </c>
-      <c r="Q20" s="89"/>
+      <c r="Q20" s="89">
+        <v>1</v>
+      </c>
       <c r="R20" s="91"/>
       <c r="S20" s="57"/>
       <c r="T20" s="58"/>
@@ -3793,7 +3795,7 @@
       </c>
       <c r="D23" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E23" s="50"/>
       <c r="F23" s="51"/>
@@ -3807,7 +3809,9 @@
       <c r="N23" s="59"/>
       <c r="O23" s="60"/>
       <c r="P23" s="61"/>
-      <c r="Q23" s="91"/>
+      <c r="Q23" s="91">
+        <v>3</v>
+      </c>
       <c r="R23" s="89"/>
       <c r="S23" s="57"/>
       <c r="T23" s="58"/>
@@ -5243,7 +5247,7 @@
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>18.25</v>
+        <v>22.25</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5289,7 +5293,7 @@
       </c>
       <c r="Q43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R43" s="39">
         <f t="shared" si="3"/>
@@ -5575,7 +5579,7 @@
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>6.25</v>
+        <v>10.25</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>

</xml_diff>

<commit_message>
Zeitplanung und Dokumentation wurden angepasst.
</commit_message>
<xml_diff>
--- a/doc/Zeitplanung.xlsx
+++ b/doc/Zeitplanung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Jump-And-Run\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8EC601A-95DD-4B9E-ADB3-126762A3ED0F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48275093-ED36-4B97-A63C-63C5673D848D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="64">
   <si>
     <t>Nr.</t>
   </si>
@@ -254,13 +254,19 @@
     <t>Anforderung F.REQ.004</t>
   </si>
   <si>
-    <t>Anforderung NF.REQ.002</t>
-  </si>
-  <si>
-    <t>Anforderung F.REQ.007</t>
-  </si>
-  <si>
     <t>Anforderung F.REQ.005</t>
+  </si>
+  <si>
+    <t>Anforderung F.REQ 007</t>
+  </si>
+  <si>
+    <t>Anforderung F.REQ 010</t>
+  </si>
+  <si>
+    <t>Anforderung F.REQ 008</t>
+  </si>
+  <si>
+    <t>Anforderung F.REQ 009</t>
   </si>
 </sst>
 </file>
@@ -270,7 +276,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
@@ -366,6 +372,13 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="10"/>
+      <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1108,7 +1121,7 @@
     </xf>
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1459,6 +1472,18 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1566,7 +1591,7 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>64.5</c:v>
+                  <c:v>59.51</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>13</c:v>
@@ -1575,7 +1600,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2147,8 +2172,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3418,7 +3443,7 @@
       </c>
       <c r="C18" s="41">
         <f>SUM(C19:C30)</f>
-        <v>64.5</v>
+        <v>59.51</v>
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
@@ -3641,7 +3666,7 @@
         <v>54</v>
       </c>
       <c r="C21" s="49">
-        <v>4.5</v>
+        <v>2.5</v>
       </c>
       <c r="D21" s="83">
         <f t="shared" si="0"/>
@@ -3718,7 +3743,7 @@
         <v>57</v>
       </c>
       <c r="C22" s="49">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="D22" s="83">
         <f t="shared" si="0"/>
@@ -3744,7 +3769,7 @@
       <c r="V22" s="60"/>
       <c r="W22" s="91"/>
       <c r="X22" s="55"/>
-      <c r="Y22" s="92"/>
+      <c r="Y22" s="104"/>
       <c r="Z22" s="57"/>
       <c r="AA22" s="58"/>
       <c r="AB22" s="54"/>
@@ -3873,9 +3898,7 @@
         <v>0</v>
       </c>
       <c r="E24" s="50"/>
-      <c r="F24" s="51" t="s">
-        <v>52</v>
-      </c>
+      <c r="F24" s="51"/>
       <c r="G24" s="59"/>
       <c r="H24" s="60"/>
       <c r="I24" s="55"/>
@@ -3894,7 +3917,7 @@
       <c r="V24" s="60"/>
       <c r="W24" s="91"/>
       <c r="X24" s="91"/>
-      <c r="Y24" s="52"/>
+      <c r="Y24" s="94"/>
       <c r="Z24" s="57"/>
       <c r="AA24" s="58"/>
       <c r="AB24" s="54"/>
@@ -3965,9 +3988,9 @@
       <c r="T25" s="58"/>
       <c r="U25" s="59"/>
       <c r="V25" s="60"/>
-      <c r="W25" s="89"/>
-      <c r="X25" s="89"/>
-      <c r="Y25" s="89"/>
+      <c r="W25" s="91"/>
+      <c r="X25" s="91"/>
+      <c r="Y25" s="91"/>
       <c r="Z25" s="57"/>
       <c r="AA25" s="58"/>
       <c r="AB25" s="54"/>
@@ -4011,17 +4034,19 @@
         <v>308</v>
       </c>
       <c r="B26" s="46" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C26" s="49">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D26" s="83">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E26" s="50"/>
-      <c r="F26" s="51"/>
+      <c r="F26" s="51" t="s">
+        <v>52</v>
+      </c>
       <c r="G26" s="59"/>
       <c r="H26" s="60"/>
       <c r="I26" s="55"/>
@@ -4039,8 +4064,8 @@
       <c r="U26" s="59"/>
       <c r="V26" s="60"/>
       <c r="W26" s="91"/>
-      <c r="X26" s="89"/>
-      <c r="Y26" s="89"/>
+      <c r="X26" s="104"/>
+      <c r="Y26" s="51"/>
       <c r="Z26" s="57"/>
       <c r="AA26" s="58"/>
       <c r="AB26" s="54"/>
@@ -4084,10 +4109,10 @@
         <v>309</v>
       </c>
       <c r="B27" s="46" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C27" s="49">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D27" s="83">
         <f t="shared" si="0"/>
@@ -4157,19 +4182,17 @@
         <v>310</v>
       </c>
       <c r="B28" s="46" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C28" s="49">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D28" s="83">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E28" s="50"/>
-      <c r="F28" s="51" t="s">
-        <v>53</v>
-      </c>
+      <c r="F28" s="51"/>
       <c r="G28" s="59"/>
       <c r="H28" s="60"/>
       <c r="I28" s="55"/>
@@ -4191,8 +4214,8 @@
       <c r="Y28" s="56"/>
       <c r="Z28" s="57"/>
       <c r="AA28" s="58"/>
-      <c r="AB28" s="89"/>
-      <c r="AC28" s="89"/>
+      <c r="AB28" s="91"/>
+      <c r="AC28" s="91"/>
       <c r="AD28" s="54"/>
       <c r="AE28" s="54"/>
       <c r="AF28" s="54"/>
@@ -4207,7 +4230,7 @@
       <c r="AO28" s="54"/>
       <c r="AP28" s="59"/>
       <c r="AQ28" s="60"/>
-      <c r="AR28" s="52"/>
+      <c r="AR28" s="105"/>
       <c r="AS28" s="55"/>
       <c r="AT28" s="56"/>
       <c r="AU28" s="57"/>
@@ -4232,17 +4255,19 @@
         <v>311</v>
       </c>
       <c r="B29" s="46" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C29" s="49">
-        <v>8</v>
+        <v>0.01</v>
       </c>
       <c r="D29" s="83">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E29" s="50"/>
-      <c r="F29" s="51"/>
+      <c r="F29" s="51" t="s">
+        <v>53</v>
+      </c>
       <c r="G29" s="71"/>
       <c r="H29" s="72"/>
       <c r="I29" s="55"/>
@@ -4280,8 +4305,8 @@
       <c r="AO29" s="54"/>
       <c r="AP29" s="71"/>
       <c r="AQ29" s="72"/>
-      <c r="AR29" s="89"/>
-      <c r="AS29" s="91"/>
+      <c r="AR29" s="51"/>
+      <c r="AS29" s="106"/>
       <c r="AT29" s="56"/>
       <c r="AU29" s="57"/>
       <c r="AV29" s="58"/>
@@ -4304,8 +4329,12 @@
       <c r="A30" s="12">
         <v>312</v>
       </c>
-      <c r="B30" s="46"/>
-      <c r="C30" s="49"/>
+      <c r="B30" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="49">
+        <v>2</v>
+      </c>
       <c r="D30" s="83">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4329,8 +4358,8 @@
       <c r="U30" s="69"/>
       <c r="V30" s="70"/>
       <c r="W30" s="55"/>
-      <c r="X30" s="55"/>
-      <c r="Y30" s="56"/>
+      <c r="X30" s="68"/>
+      <c r="Y30" s="63"/>
       <c r="Z30" s="57"/>
       <c r="AA30" s="58"/>
       <c r="AB30" s="54"/>
@@ -4956,7 +4985,7 @@
       </c>
       <c r="C39" s="41">
         <f>SUM(C40:C42)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D39" s="42">
         <f>SUM(D40:D42)</f>
@@ -5029,7 +5058,7 @@
         <v>31</v>
       </c>
       <c r="C40" s="49">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D40" s="83">
         <f>SUM(G40:BJ40)</f>
@@ -5243,7 +5272,7 @@
       </c>
       <c r="C43" s="37">
         <f>C39+C36+C31+C18+C14+C9</f>
-        <v>112.5</v>
+        <v>106.50999999999999</v>
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
@@ -5575,7 +5604,7 @@
       <c r="B5" s="101"/>
       <c r="C5" s="80">
         <f>Zeitplanung!C18</f>
-        <v>64.5</v>
+        <v>59.51</v>
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
@@ -5624,7 +5653,7 @@
       <c r="B8" s="101"/>
       <c r="C8" s="80">
         <f>Zeitplanung!C39</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" s="80">
         <f>Zeitplanung!D39</f>

</xml_diff>

<commit_message>
Timer wurde hinzugefügt, dieser kann allerdings noch nicht ausgelesen werden.
</commit_message>
<xml_diff>
--- a/doc/Zeitplanung.xlsx
+++ b/doc/Zeitplanung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Jump-And-Run\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48275093-ED36-4B97-A63C-63C5673D848D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E470735F-15F2-420B-AF4C-5BAAB12598F2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1442,6 +1442,18 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1472,18 +1484,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1659,13 +1659,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.25</c:v>
+                  <c:v>17.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2172,8 +2172,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="V22" sqref="V22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2492,88 +2492,88 @@
     <row r="7" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
       <c r="B7" s="27"/>
-      <c r="C7" s="95" t="s">
+      <c r="C7" s="98" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="95"/>
+      <c r="D7" s="98"/>
       <c r="E7" s="28" t="s">
         <v>21</v>
       </c>
       <c r="F7" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="96" t="s">
+      <c r="G7" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="96"/>
-      <c r="I7" s="96"/>
-      <c r="J7" s="96"/>
-      <c r="K7" s="96"/>
-      <c r="L7" s="96"/>
-      <c r="M7" s="97"/>
-      <c r="N7" s="96" t="s">
+      <c r="H7" s="99"/>
+      <c r="I7" s="99"/>
+      <c r="J7" s="99"/>
+      <c r="K7" s="99"/>
+      <c r="L7" s="99"/>
+      <c r="M7" s="100"/>
+      <c r="N7" s="99" t="s">
         <v>37</v>
       </c>
-      <c r="O7" s="96"/>
-      <c r="P7" s="96"/>
-      <c r="Q7" s="96"/>
-      <c r="R7" s="96"/>
-      <c r="S7" s="96"/>
-      <c r="T7" s="97"/>
-      <c r="U7" s="96" t="s">
+      <c r="O7" s="99"/>
+      <c r="P7" s="99"/>
+      <c r="Q7" s="99"/>
+      <c r="R7" s="99"/>
+      <c r="S7" s="99"/>
+      <c r="T7" s="100"/>
+      <c r="U7" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="V7" s="96"/>
-      <c r="W7" s="96"/>
-      <c r="X7" s="96"/>
-      <c r="Y7" s="96"/>
-      <c r="Z7" s="96"/>
-      <c r="AA7" s="97"/>
-      <c r="AB7" s="98" t="s">
+      <c r="V7" s="99"/>
+      <c r="W7" s="99"/>
+      <c r="X7" s="99"/>
+      <c r="Y7" s="99"/>
+      <c r="Z7" s="99"/>
+      <c r="AA7" s="100"/>
+      <c r="AB7" s="101" t="s">
         <v>39</v>
       </c>
-      <c r="AC7" s="96"/>
-      <c r="AD7" s="96"/>
-      <c r="AE7" s="96"/>
-      <c r="AF7" s="96"/>
-      <c r="AG7" s="96"/>
-      <c r="AH7" s="97"/>
-      <c r="AI7" s="96" t="s">
+      <c r="AC7" s="99"/>
+      <c r="AD7" s="99"/>
+      <c r="AE7" s="99"/>
+      <c r="AF7" s="99"/>
+      <c r="AG7" s="99"/>
+      <c r="AH7" s="100"/>
+      <c r="AI7" s="99" t="s">
         <v>40</v>
       </c>
-      <c r="AJ7" s="96"/>
-      <c r="AK7" s="96"/>
-      <c r="AL7" s="96"/>
-      <c r="AM7" s="96"/>
-      <c r="AN7" s="96"/>
-      <c r="AO7" s="97"/>
-      <c r="AP7" s="98" t="s">
+      <c r="AJ7" s="99"/>
+      <c r="AK7" s="99"/>
+      <c r="AL7" s="99"/>
+      <c r="AM7" s="99"/>
+      <c r="AN7" s="99"/>
+      <c r="AO7" s="100"/>
+      <c r="AP7" s="101" t="s">
         <v>41</v>
       </c>
-      <c r="AQ7" s="96"/>
-      <c r="AR7" s="96"/>
-      <c r="AS7" s="96"/>
-      <c r="AT7" s="96"/>
-      <c r="AU7" s="96"/>
-      <c r="AV7" s="97"/>
-      <c r="AW7" s="96" t="s">
+      <c r="AQ7" s="99"/>
+      <c r="AR7" s="99"/>
+      <c r="AS7" s="99"/>
+      <c r="AT7" s="99"/>
+      <c r="AU7" s="99"/>
+      <c r="AV7" s="100"/>
+      <c r="AW7" s="99" t="s">
         <v>42</v>
       </c>
-      <c r="AX7" s="96"/>
-      <c r="AY7" s="96"/>
-      <c r="AZ7" s="96"/>
-      <c r="BA7" s="96"/>
-      <c r="BB7" s="96"/>
-      <c r="BC7" s="97"/>
-      <c r="BD7" s="98" t="s">
+      <c r="AX7" s="99"/>
+      <c r="AY7" s="99"/>
+      <c r="AZ7" s="99"/>
+      <c r="BA7" s="99"/>
+      <c r="BB7" s="99"/>
+      <c r="BC7" s="100"/>
+      <c r="BD7" s="101" t="s">
         <v>43</v>
       </c>
-      <c r="BE7" s="96"/>
-      <c r="BF7" s="96"/>
-      <c r="BG7" s="96"/>
-      <c r="BH7" s="96"/>
-      <c r="BI7" s="96"/>
-      <c r="BJ7" s="99"/>
+      <c r="BE7" s="99"/>
+      <c r="BF7" s="99"/>
+      <c r="BG7" s="99"/>
+      <c r="BH7" s="99"/>
+      <c r="BI7" s="99"/>
+      <c r="BJ7" s="102"/>
     </row>
     <row r="8" spans="1:62" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
@@ -2774,7 +2774,7 @@
       </c>
       <c r="D9" s="42">
         <f>SUM(D10:D13)</f>
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="E9" s="32"/>
       <c r="F9" s="31"/>
@@ -2998,7 +2998,7 @@
       </c>
       <c r="D12" s="83">
         <f>SUM(G12:BJ12)</f>
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="E12" s="50">
         <v>1</v>
@@ -3017,7 +3017,9 @@
       <c r="O12" s="60"/>
       <c r="P12" s="61"/>
       <c r="Q12" s="61"/>
-      <c r="R12" s="63"/>
+      <c r="R12" s="63">
+        <v>1.5</v>
+      </c>
       <c r="S12" s="57"/>
       <c r="T12" s="58"/>
       <c r="U12" s="59"/>
@@ -3447,7 +3449,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>10.25</v>
+        <v>17.25</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3670,7 +3672,7 @@
       </c>
       <c r="D21" s="83">
         <f t="shared" si="0"/>
-        <v>4.25</v>
+        <v>4.75</v>
       </c>
       <c r="E21" s="50"/>
       <c r="F21" s="52" t="s">
@@ -3688,7 +3690,9 @@
       <c r="P21" s="93">
         <v>4.25</v>
       </c>
-      <c r="Q21" s="89"/>
+      <c r="Q21" s="89">
+        <v>0.5</v>
+      </c>
       <c r="R21" s="52"/>
       <c r="S21" s="57"/>
       <c r="T21" s="58"/>
@@ -3747,7 +3751,7 @@
       </c>
       <c r="D22" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E22" s="50"/>
       <c r="F22" s="51"/>
@@ -3761,7 +3765,9 @@
       <c r="N22" s="59"/>
       <c r="O22" s="60"/>
       <c r="P22" s="55"/>
-      <c r="Q22" s="89"/>
+      <c r="Q22" s="89">
+        <v>0.5</v>
+      </c>
       <c r="R22" s="91"/>
       <c r="S22" s="57"/>
       <c r="T22" s="58"/>
@@ -3769,7 +3775,7 @@
       <c r="V22" s="60"/>
       <c r="W22" s="91"/>
       <c r="X22" s="55"/>
-      <c r="Y22" s="104"/>
+      <c r="Y22" s="95"/>
       <c r="Z22" s="57"/>
       <c r="AA22" s="58"/>
       <c r="AB22" s="54"/>
@@ -3820,7 +3826,7 @@
       </c>
       <c r="D23" s="83">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="E23" s="50"/>
       <c r="F23" s="51"/>
@@ -3835,9 +3841,11 @@
       <c r="O23" s="60"/>
       <c r="P23" s="61"/>
       <c r="Q23" s="91">
-        <v>3</v>
-      </c>
-      <c r="R23" s="89"/>
+        <v>2.5</v>
+      </c>
+      <c r="R23" s="89">
+        <v>1</v>
+      </c>
       <c r="S23" s="57"/>
       <c r="T23" s="58"/>
       <c r="U23" s="59"/>
@@ -3895,7 +3903,7 @@
       </c>
       <c r="D24" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E24" s="50"/>
       <c r="F24" s="51"/>
@@ -3909,8 +3917,12 @@
       <c r="N24" s="59"/>
       <c r="O24" s="60"/>
       <c r="P24" s="55"/>
-      <c r="Q24" s="91"/>
-      <c r="R24" s="89"/>
+      <c r="Q24" s="91">
+        <v>1.5</v>
+      </c>
+      <c r="R24" s="89">
+        <v>0.5</v>
+      </c>
       <c r="S24" s="57"/>
       <c r="T24" s="58"/>
       <c r="U24" s="59"/>
@@ -3968,7 +3980,7 @@
       </c>
       <c r="D25" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="E25" s="50"/>
       <c r="F25" s="51"/>
@@ -3983,7 +3995,9 @@
       <c r="O25" s="60"/>
       <c r="P25" s="55"/>
       <c r="Q25" s="55"/>
-      <c r="R25" s="56"/>
+      <c r="R25" s="91">
+        <v>3.5</v>
+      </c>
       <c r="S25" s="57"/>
       <c r="T25" s="58"/>
       <c r="U25" s="59"/>
@@ -4063,8 +4077,8 @@
       <c r="T26" s="58"/>
       <c r="U26" s="59"/>
       <c r="V26" s="60"/>
-      <c r="W26" s="91"/>
-      <c r="X26" s="104"/>
+      <c r="W26" s="95"/>
+      <c r="X26" s="95"/>
       <c r="Y26" s="51"/>
       <c r="Z26" s="57"/>
       <c r="AA26" s="58"/>
@@ -4230,7 +4244,7 @@
       <c r="AO28" s="54"/>
       <c r="AP28" s="59"/>
       <c r="AQ28" s="60"/>
-      <c r="AR28" s="105"/>
+      <c r="AR28" s="96"/>
       <c r="AS28" s="55"/>
       <c r="AT28" s="56"/>
       <c r="AU28" s="57"/>
@@ -4306,7 +4320,7 @@
       <c r="AP29" s="71"/>
       <c r="AQ29" s="72"/>
       <c r="AR29" s="51"/>
-      <c r="AS29" s="106"/>
+      <c r="AS29" s="97"/>
       <c r="AT29" s="56"/>
       <c r="AU29" s="57"/>
       <c r="AV29" s="58"/>
@@ -5276,7 +5290,7 @@
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>22.25</v>
+        <v>30.75</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5322,11 +5336,11 @@
       </c>
       <c r="Q43" s="39">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="R43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="S43" s="39">
         <f t="shared" si="3"/>
@@ -5551,10 +5565,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="103"/>
+      <c r="B2" s="106"/>
       <c r="C2" s="79" t="s">
         <v>14</v>
       </c>
@@ -5563,28 +5577,28 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="100" t="str">
+      <c r="A3" s="103" t="str">
         <f>Zeitplanung!B9</f>
         <v>Administration, Planung</v>
       </c>
-      <c r="B3" s="101"/>
+      <c r="B3" s="104"/>
       <c r="C3" s="80">
         <f>Zeitplanung!C9</f>
         <v>5</v>
       </c>
       <c r="D3" s="80">
         <f>Zeitplanung!D9</f>
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="E3" s="82"/>
       <c r="F3" s="81"/>
     </row>
     <row r="4" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="100" t="str">
+      <c r="A4" s="103" t="str">
         <f>Zeitplanung!B14</f>
         <v>Analyse &amp; Design</v>
       </c>
-      <c r="B4" s="101"/>
+      <c r="B4" s="104"/>
       <c r="C4" s="80">
         <f>Zeitplanung!C14</f>
         <v>12</v>
@@ -5597,28 +5611,28 @@
       <c r="F4" s="81"/>
     </row>
     <row r="5" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="100" t="str">
+      <c r="A5" s="103" t="str">
         <f>Zeitplanung!B18</f>
         <v>Implementation</v>
       </c>
-      <c r="B5" s="101"/>
+      <c r="B5" s="104"/>
       <c r="C5" s="80">
         <f>Zeitplanung!C18</f>
         <v>59.51</v>
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>10.25</v>
+        <v>17.25</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>
     </row>
     <row r="6" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="100" t="str">
+      <c r="A6" s="103" t="str">
         <f>Zeitplanung!B31</f>
         <v>Testen</v>
       </c>
-      <c r="B6" s="101"/>
+      <c r="B6" s="104"/>
       <c r="C6" s="80">
         <f>Zeitplanung!C31</f>
         <v>13</v>
@@ -5630,11 +5644,11 @@
       <c r="F6" s="81"/>
     </row>
     <row r="7" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="100" t="str">
+      <c r="A7" s="103" t="str">
         <f>Zeitplanung!B36</f>
         <v>Diverses</v>
       </c>
-      <c r="B7" s="101"/>
+      <c r="B7" s="104"/>
       <c r="C7" s="80">
         <f>Zeitplanung!C36</f>
         <v>10</v>
@@ -5646,11 +5660,11 @@
       <c r="F7" s="81"/>
     </row>
     <row r="8" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="100" t="str">
+      <c r="A8" s="103" t="str">
         <f>Zeitplanung!B39</f>
         <v>Abschluss</v>
       </c>
-      <c r="B8" s="101"/>
+      <c r="B8" s="104"/>
       <c r="C8" s="80">
         <f>Zeitplanung!C39</f>
         <v>7</v>

</xml_diff>

<commit_message>
Stopwatch wurde hinzugefügt und wird auf neue Webseite übergeben. Allerdings können die Daten noch nicht auf die Datenbank hochgeladen werden.
Das Zeichnen der Hindernisse wurde verbessert.
</commit_message>
<xml_diff>
--- a/doc/Zeitplanung.xlsx
+++ b/doc/Zeitplanung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Jump-And-Run\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E470735F-15F2-420B-AF4C-5BAAB12598F2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F385B9-7012-4AC3-8740-EB7EE3D7C438}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1665,7 +1665,7 @@
                   <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.25</c:v>
+                  <c:v>23.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2172,8 +2172,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="V22" sqref="V22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AI24" sqref="AI24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3449,7 +3449,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>17.25</v>
+        <v>23.75</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3773,8 +3773,8 @@
       <c r="T22" s="58"/>
       <c r="U22" s="59"/>
       <c r="V22" s="60"/>
-      <c r="W22" s="91"/>
-      <c r="X22" s="55"/>
+      <c r="W22" s="95"/>
+      <c r="X22" s="95"/>
       <c r="Y22" s="95"/>
       <c r="Z22" s="57"/>
       <c r="AA22" s="58"/>
@@ -3826,7 +3826,7 @@
       </c>
       <c r="D23" s="83">
         <f t="shared" si="0"/>
-        <v>3.5</v>
+        <v>8</v>
       </c>
       <c r="E23" s="50"/>
       <c r="F23" s="51"/>
@@ -3850,7 +3850,9 @@
       <c r="T23" s="58"/>
       <c r="U23" s="59"/>
       <c r="V23" s="60"/>
-      <c r="W23" s="91"/>
+      <c r="W23" s="91">
+        <v>4.5</v>
+      </c>
       <c r="X23" s="91"/>
       <c r="Y23" s="91"/>
       <c r="Z23" s="57"/>
@@ -3980,7 +3982,7 @@
       </c>
       <c r="D25" s="83">
         <f t="shared" si="0"/>
-        <v>3.5</v>
+        <v>5.5</v>
       </c>
       <c r="E25" s="50"/>
       <c r="F25" s="51"/>
@@ -4002,7 +4004,9 @@
       <c r="T25" s="58"/>
       <c r="U25" s="59"/>
       <c r="V25" s="60"/>
-      <c r="W25" s="91"/>
+      <c r="W25" s="91">
+        <v>2</v>
+      </c>
       <c r="X25" s="91"/>
       <c r="Y25" s="91"/>
       <c r="Z25" s="57"/>
@@ -4077,7 +4081,7 @@
       <c r="T26" s="58"/>
       <c r="U26" s="59"/>
       <c r="V26" s="60"/>
-      <c r="W26" s="95"/>
+      <c r="W26" s="92"/>
       <c r="X26" s="95"/>
       <c r="Y26" s="51"/>
       <c r="Z26" s="57"/>
@@ -5290,7 +5294,7 @@
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>30.75</v>
+        <v>37.25</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5360,7 +5364,7 @@
       </c>
       <c r="W43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="X43" s="39">
         <f t="shared" si="3"/>
@@ -5622,7 +5626,7 @@
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>17.25</v>
+        <v>23.75</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>

</xml_diff>

<commit_message>
Ein kleines Anti-Cheat wurde eingebaut um Benutzern das Schummeln durch manipulieren der URL zu erschweren
</commit_message>
<xml_diff>
--- a/doc/Zeitplanung.xlsx
+++ b/doc/Zeitplanung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Jump-And-Run\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F385B9-7012-4AC3-8740-EB7EE3D7C438}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45328AE5-E056-49B3-AD26-56FBA1BF0AC2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1121,7 +1121,7 @@
     </xf>
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1439,10 +1439,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1659,13 +1655,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.75</c:v>
+                  <c:v>36.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2173,7 +2169,7 @@
   <dimension ref="A1:BJ43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AI24" sqref="AI24"/>
+      <selection activeCell="Z22" sqref="Z22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2492,88 +2488,88 @@
     <row r="7" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
       <c r="B7" s="27"/>
-      <c r="C7" s="98" t="s">
+      <c r="C7" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="98"/>
+      <c r="D7" s="97"/>
       <c r="E7" s="28" t="s">
         <v>21</v>
       </c>
       <c r="F7" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="99" t="s">
+      <c r="G7" s="98" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="99"/>
-      <c r="I7" s="99"/>
-      <c r="J7" s="99"/>
-      <c r="K7" s="99"/>
-      <c r="L7" s="99"/>
-      <c r="M7" s="100"/>
-      <c r="N7" s="99" t="s">
+      <c r="H7" s="98"/>
+      <c r="I7" s="98"/>
+      <c r="J7" s="98"/>
+      <c r="K7" s="98"/>
+      <c r="L7" s="98"/>
+      <c r="M7" s="99"/>
+      <c r="N7" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="O7" s="99"/>
-      <c r="P7" s="99"/>
-      <c r="Q7" s="99"/>
-      <c r="R7" s="99"/>
-      <c r="S7" s="99"/>
-      <c r="T7" s="100"/>
-      <c r="U7" s="99" t="s">
+      <c r="O7" s="98"/>
+      <c r="P7" s="98"/>
+      <c r="Q7" s="98"/>
+      <c r="R7" s="98"/>
+      <c r="S7" s="98"/>
+      <c r="T7" s="99"/>
+      <c r="U7" s="98" t="s">
         <v>38</v>
       </c>
-      <c r="V7" s="99"/>
-      <c r="W7" s="99"/>
-      <c r="X7" s="99"/>
-      <c r="Y7" s="99"/>
-      <c r="Z7" s="99"/>
-      <c r="AA7" s="100"/>
-      <c r="AB7" s="101" t="s">
+      <c r="V7" s="98"/>
+      <c r="W7" s="98"/>
+      <c r="X7" s="98"/>
+      <c r="Y7" s="98"/>
+      <c r="Z7" s="98"/>
+      <c r="AA7" s="99"/>
+      <c r="AB7" s="100" t="s">
         <v>39</v>
       </c>
-      <c r="AC7" s="99"/>
-      <c r="AD7" s="99"/>
-      <c r="AE7" s="99"/>
-      <c r="AF7" s="99"/>
-      <c r="AG7" s="99"/>
-      <c r="AH7" s="100"/>
-      <c r="AI7" s="99" t="s">
+      <c r="AC7" s="98"/>
+      <c r="AD7" s="98"/>
+      <c r="AE7" s="98"/>
+      <c r="AF7" s="98"/>
+      <c r="AG7" s="98"/>
+      <c r="AH7" s="99"/>
+      <c r="AI7" s="98" t="s">
         <v>40</v>
       </c>
-      <c r="AJ7" s="99"/>
-      <c r="AK7" s="99"/>
-      <c r="AL7" s="99"/>
-      <c r="AM7" s="99"/>
-      <c r="AN7" s="99"/>
-      <c r="AO7" s="100"/>
-      <c r="AP7" s="101" t="s">
+      <c r="AJ7" s="98"/>
+      <c r="AK7" s="98"/>
+      <c r="AL7" s="98"/>
+      <c r="AM7" s="98"/>
+      <c r="AN7" s="98"/>
+      <c r="AO7" s="99"/>
+      <c r="AP7" s="100" t="s">
         <v>41</v>
       </c>
-      <c r="AQ7" s="99"/>
-      <c r="AR7" s="99"/>
-      <c r="AS7" s="99"/>
-      <c r="AT7" s="99"/>
-      <c r="AU7" s="99"/>
-      <c r="AV7" s="100"/>
-      <c r="AW7" s="99" t="s">
+      <c r="AQ7" s="98"/>
+      <c r="AR7" s="98"/>
+      <c r="AS7" s="98"/>
+      <c r="AT7" s="98"/>
+      <c r="AU7" s="98"/>
+      <c r="AV7" s="99"/>
+      <c r="AW7" s="98" t="s">
         <v>42</v>
       </c>
-      <c r="AX7" s="99"/>
-      <c r="AY7" s="99"/>
-      <c r="AZ7" s="99"/>
-      <c r="BA7" s="99"/>
-      <c r="BB7" s="99"/>
-      <c r="BC7" s="100"/>
-      <c r="BD7" s="101" t="s">
+      <c r="AX7" s="98"/>
+      <c r="AY7" s="98"/>
+      <c r="AZ7" s="98"/>
+      <c r="BA7" s="98"/>
+      <c r="BB7" s="98"/>
+      <c r="BC7" s="99"/>
+      <c r="BD7" s="100" t="s">
         <v>43</v>
       </c>
-      <c r="BE7" s="99"/>
-      <c r="BF7" s="99"/>
-      <c r="BG7" s="99"/>
-      <c r="BH7" s="99"/>
-      <c r="BI7" s="99"/>
-      <c r="BJ7" s="102"/>
+      <c r="BE7" s="98"/>
+      <c r="BF7" s="98"/>
+      <c r="BG7" s="98"/>
+      <c r="BH7" s="98"/>
+      <c r="BI7" s="98"/>
+      <c r="BJ7" s="101"/>
     </row>
     <row r="8" spans="1:62" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
@@ -2774,7 +2770,7 @@
       </c>
       <c r="D9" s="42">
         <f>SUM(D10:D13)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E9" s="32"/>
       <c r="F9" s="31"/>
@@ -2998,7 +2994,7 @@
       </c>
       <c r="D12" s="83">
         <f>SUM(G12:BJ12)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E12" s="50">
         <v>1</v>
@@ -3026,7 +3022,9 @@
       <c r="V12" s="60"/>
       <c r="W12" s="61"/>
       <c r="X12" s="61"/>
-      <c r="Y12" s="63"/>
+      <c r="Y12" s="63">
+        <v>1</v>
+      </c>
       <c r="Z12" s="57"/>
       <c r="AA12" s="58"/>
       <c r="AB12" s="54"/>
@@ -3449,7 +3447,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>23.75</v>
+        <v>36.75</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3751,7 +3749,7 @@
       </c>
       <c r="D22" s="83">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>14</v>
       </c>
       <c r="E22" s="50"/>
       <c r="F22" s="51"/>
@@ -3773,9 +3771,15 @@
       <c r="T22" s="58"/>
       <c r="U22" s="59"/>
       <c r="V22" s="60"/>
-      <c r="W22" s="95"/>
-      <c r="X22" s="95"/>
-      <c r="Y22" s="95"/>
+      <c r="W22" s="89">
+        <v>4.5</v>
+      </c>
+      <c r="X22" s="89">
+        <v>3</v>
+      </c>
+      <c r="Y22" s="89">
+        <v>6</v>
+      </c>
       <c r="Z22" s="57"/>
       <c r="AA22" s="58"/>
       <c r="AB22" s="54"/>
@@ -3826,7 +3830,7 @@
       </c>
       <c r="D23" s="83">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>3.5</v>
       </c>
       <c r="E23" s="50"/>
       <c r="F23" s="51"/>
@@ -3850,10 +3854,8 @@
       <c r="T23" s="58"/>
       <c r="U23" s="59"/>
       <c r="V23" s="60"/>
-      <c r="W23" s="91">
-        <v>4.5</v>
-      </c>
-      <c r="X23" s="91"/>
+      <c r="W23" s="91"/>
+      <c r="X23" s="92"/>
       <c r="Y23" s="91"/>
       <c r="Z23" s="57"/>
       <c r="AA23" s="58"/>
@@ -4059,7 +4061,7 @@
       </c>
       <c r="D26" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E26" s="50"/>
       <c r="F26" s="51" t="s">
@@ -4082,7 +4084,9 @@
       <c r="U26" s="59"/>
       <c r="V26" s="60"/>
       <c r="W26" s="92"/>
-      <c r="X26" s="95"/>
+      <c r="X26" s="89">
+        <v>4</v>
+      </c>
       <c r="Y26" s="51"/>
       <c r="Z26" s="57"/>
       <c r="AA26" s="58"/>
@@ -4248,7 +4252,7 @@
       <c r="AO28" s="54"/>
       <c r="AP28" s="59"/>
       <c r="AQ28" s="60"/>
-      <c r="AR28" s="96"/>
+      <c r="AR28" s="95"/>
       <c r="AS28" s="55"/>
       <c r="AT28" s="56"/>
       <c r="AU28" s="57"/>
@@ -4324,7 +4328,7 @@
       <c r="AP29" s="71"/>
       <c r="AQ29" s="72"/>
       <c r="AR29" s="51"/>
-      <c r="AS29" s="97"/>
+      <c r="AS29" s="96"/>
       <c r="AT29" s="56"/>
       <c r="AU29" s="57"/>
       <c r="AV29" s="58"/>
@@ -5294,7 +5298,7 @@
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>37.25</v>
+        <v>51.25</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5368,11 +5372,11 @@
       </c>
       <c r="X43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Y43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Z43" s="39">
         <f t="shared" si="3"/>
@@ -5569,10 +5573,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="105" t="s">
+      <c r="A2" s="104" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="106"/>
+      <c r="B2" s="105"/>
       <c r="C2" s="79" t="s">
         <v>14</v>
       </c>
@@ -5581,28 +5585,28 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="103" t="str">
+      <c r="A3" s="102" t="str">
         <f>Zeitplanung!B9</f>
         <v>Administration, Planung</v>
       </c>
-      <c r="B3" s="104"/>
+      <c r="B3" s="103"/>
       <c r="C3" s="80">
         <f>Zeitplanung!C9</f>
         <v>5</v>
       </c>
       <c r="D3" s="80">
         <f>Zeitplanung!D9</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E3" s="82"/>
       <c r="F3" s="81"/>
     </row>
     <row r="4" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="103" t="str">
+      <c r="A4" s="102" t="str">
         <f>Zeitplanung!B14</f>
         <v>Analyse &amp; Design</v>
       </c>
-      <c r="B4" s="104"/>
+      <c r="B4" s="103"/>
       <c r="C4" s="80">
         <f>Zeitplanung!C14</f>
         <v>12</v>
@@ -5615,28 +5619,28 @@
       <c r="F4" s="81"/>
     </row>
     <row r="5" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="103" t="str">
+      <c r="A5" s="102" t="str">
         <f>Zeitplanung!B18</f>
         <v>Implementation</v>
       </c>
-      <c r="B5" s="104"/>
+      <c r="B5" s="103"/>
       <c r="C5" s="80">
         <f>Zeitplanung!C18</f>
         <v>59.51</v>
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>23.75</v>
+        <v>36.75</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>
     </row>
     <row r="6" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="103" t="str">
+      <c r="A6" s="102" t="str">
         <f>Zeitplanung!B31</f>
         <v>Testen</v>
       </c>
-      <c r="B6" s="104"/>
+      <c r="B6" s="103"/>
       <c r="C6" s="80">
         <f>Zeitplanung!C31</f>
         <v>13</v>
@@ -5648,11 +5652,11 @@
       <c r="F6" s="81"/>
     </row>
     <row r="7" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="103" t="str">
+      <c r="A7" s="102" t="str">
         <f>Zeitplanung!B36</f>
         <v>Diverses</v>
       </c>
-      <c r="B7" s="104"/>
+      <c r="B7" s="103"/>
       <c r="C7" s="80">
         <f>Zeitplanung!C36</f>
         <v>10</v>
@@ -5664,11 +5668,11 @@
       <c r="F7" s="81"/>
     </row>
     <row r="8" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="103" t="str">
+      <c r="A8" s="102" t="str">
         <f>Zeitplanung!B39</f>
         <v>Abschluss</v>
       </c>
-      <c r="B8" s="104"/>
+      <c r="B8" s="103"/>
       <c r="C8" s="80">
         <f>Zeitplanung!C39</f>
         <v>7</v>

</xml_diff>

<commit_message>
Ein weiters Level sowie das dazugehörende Scoreboard wurde hinzugefügt.
</commit_message>
<xml_diff>
--- a/doc/Zeitplanung.xlsx
+++ b/doc/Zeitplanung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Jump-And-Run\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45328AE5-E056-49B3-AD26-56FBA1BF0AC2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C83D7C-D98B-4E19-A2E1-38F7F1A76C6E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1661,7 +1661,7 @@
                   <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.75</c:v>
+                  <c:v>44.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2168,8 +2168,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="Z22" sqref="Z22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B11" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AU11" sqref="AU1:AU1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3447,7 +3447,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>36.75</v>
+        <v>44.25</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -4138,7 +4138,7 @@
       </c>
       <c r="D27" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="E27" s="50"/>
       <c r="F27" s="51"/>
@@ -4179,7 +4179,9 @@
       <c r="AO27" s="54"/>
       <c r="AP27" s="59"/>
       <c r="AQ27" s="60"/>
-      <c r="AR27" s="55"/>
+      <c r="AR27" s="95">
+        <v>7.5</v>
+      </c>
       <c r="AS27" s="55"/>
       <c r="AT27" s="56"/>
       <c r="AU27" s="57"/>
@@ -4252,7 +4254,7 @@
       <c r="AO28" s="54"/>
       <c r="AP28" s="59"/>
       <c r="AQ28" s="60"/>
-      <c r="AR28" s="95"/>
+      <c r="AR28" s="94"/>
       <c r="AS28" s="55"/>
       <c r="AT28" s="56"/>
       <c r="AU28" s="57"/>
@@ -5298,7 +5300,7 @@
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>51.25</v>
+        <v>58.75</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5452,7 +5454,7 @@
       </c>
       <c r="AR43" s="39">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="AS43" s="39">
         <f t="shared" si="4"/>
@@ -5630,7 +5632,7 @@
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>36.75</v>
+        <v>44.25</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>

</xml_diff>